<commit_message>
TRAS 2 SEGUNDA REVISION DELIM, TODO EN PRODUCCION
</commit_message>
<xml_diff>
--- a/101-200.xlsx
+++ b/101-200.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2cd06d07815cea4/Escritorio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\TFG\app-gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29D413E1-6210-45D8-A2C8-3C0D98114614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062BAC70-3AA8-4371-B195-2EA8BE2BDA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22AB2656-C54A-4407-8881-FE3E35CF001E}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -70,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="253">
   <si>
     <t>0057815</t>
   </si>
@@ -720,9 +718,6 @@
     <t>BALDA LINEAL DE VENTA</t>
   </si>
   <si>
-    <t>0,0,0,,0</t>
-  </si>
-  <si>
     <t>0079716</t>
   </si>
   <si>
@@ -826,6 +821,12 @@
   </si>
   <si>
     <t xml:space="preserve">OBSERVACIONES </t>
+  </si>
+  <si>
+    <t>comprobado</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -835,7 +836,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1331,38 +1332,41 @@
   <dimension ref="B1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="5.25" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
     <col min="3" max="3" width="47" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" s="5" customFormat="1" ht="28.5" customHeight="1">
       <c r="B1" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="5" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1382,8 +1386,11 @@
       <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1401,8 +1408,11 @@
       <c r="G3" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1419,8 +1429,11 @@
       <c r="G4" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1440,8 +1453,11 @@
       <c r="G5" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1460,8 +1476,11 @@
       <c r="G6" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1481,8 +1500,11 @@
       <c r="G7" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1501,8 +1523,11 @@
       <c r="G8" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1519,8 +1544,11 @@
       <c r="G9" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1540,8 +1568,11 @@
       <c r="G10" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B11" s="1" t="s">
         <v>26</v>
       </c>
@@ -1561,8 +1592,11 @@
       <c r="G11" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B12" s="7" t="s">
         <v>30</v>
       </c>
@@ -1579,11 +1613,13 @@
       <c r="G12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="10"/>
+      <c r="H12" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B13" s="11" t="s">
         <v>32</v>
       </c>
@@ -1601,11 +1637,13 @@
       <c r="G13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B14" s="11" t="s">
         <v>32</v>
       </c>
@@ -1623,8 +1661,11 @@
       <c r="G14" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B15" s="11" t="s">
         <v>34</v>
       </c>
@@ -1644,8 +1685,11 @@
       <c r="G15" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1664,8 +1708,11 @@
       <c r="G16" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B17" s="11" t="s">
         <v>34</v>
       </c>
@@ -1685,8 +1732,11 @@
       <c r="G17" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -1704,8 +1754,11 @@
       <c r="G18" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B19" s="11" t="s">
         <v>38</v>
       </c>
@@ -1725,8 +1778,11 @@
       <c r="G19" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
@@ -1743,8 +1799,11 @@
       <c r="G20" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
@@ -1761,8 +1820,11 @@
       <c r="G21" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B22" s="1" t="s">
         <v>46</v>
       </c>
@@ -1780,8 +1842,11 @@
       <c r="G22" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B23" s="1" t="s">
         <v>48</v>
       </c>
@@ -1799,8 +1864,11 @@
       <c r="G23" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B24" s="1" t="s">
         <v>50</v>
       </c>
@@ -1820,8 +1888,11 @@
       <c r="G24" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B25" s="1" t="s">
         <v>52</v>
       </c>
@@ -1838,8 +1909,11 @@
       <c r="G25" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B26" s="1" t="s">
         <v>55</v>
       </c>
@@ -1856,8 +1930,11 @@
       <c r="G26" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B27" s="1" t="s">
         <v>58</v>
       </c>
@@ -1876,8 +1953,11 @@
       <c r="G27" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H27" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B28" s="7" t="s">
         <v>63</v>
       </c>
@@ -1896,8 +1976,11 @@
       <c r="G28" s="6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B29" s="14" t="s">
         <v>67</v>
       </c>
@@ -1915,8 +1998,11 @@
       <c r="G29" s="6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B30" s="1" t="s">
         <v>71</v>
       </c>
@@ -1935,8 +2021,11 @@
       <c r="G30" s="6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B31" s="7" t="s">
         <v>74</v>
       </c>
@@ -1955,8 +2044,11 @@
       <c r="G31" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B32" s="1" t="s">
         <v>76</v>
       </c>
@@ -1975,8 +2067,11 @@
       <c r="G32" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B33" s="1" t="s">
         <v>79</v>
       </c>
@@ -1995,8 +2090,11 @@
       <c r="G33" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B34" s="7" t="s">
         <v>83</v>
       </c>
@@ -2013,8 +2111,11 @@
         <v>10</v>
       </c>
       <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B35" s="7" t="s">
         <v>86</v>
       </c>
@@ -2033,8 +2134,11 @@
       <c r="G35" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="36" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B36" s="1" t="s">
         <v>88</v>
       </c>
@@ -2051,8 +2155,11 @@
       <c r="G36" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B37" s="1" t="s">
         <v>89</v>
       </c>
@@ -2072,8 +2179,11 @@
       <c r="G37" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B38" s="1" t="s">
         <v>89</v>
       </c>
@@ -2093,8 +2203,11 @@
       <c r="G38" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="2:7" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B39" s="1" t="s">
         <v>92</v>
       </c>
@@ -2114,8 +2227,11 @@
       <c r="G39" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="2:7" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B40" s="11" t="s">
         <v>94</v>
       </c>
@@ -2135,8 +2251,11 @@
       <c r="G40" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B41" s="1" t="s">
         <v>96</v>
       </c>
@@ -2153,8 +2272,11 @@
       <c r="G41" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="2:7" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B42" s="1" t="s">
         <v>99</v>
       </c>
@@ -2171,8 +2293,11 @@
       <c r="G42" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="2:7" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B43" s="1" t="s">
         <v>101</v>
       </c>
@@ -2189,8 +2314,11 @@
       <c r="G43" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="2:7" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B44" s="1" t="s">
         <v>103</v>
       </c>
@@ -2207,8 +2335,11 @@
       <c r="G44" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="45" spans="2:7" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B45" s="1" t="s">
         <v>105</v>
       </c>
@@ -2225,8 +2356,11 @@
       <c r="G45" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="2:7" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B46" s="1" t="s">
         <v>107</v>
       </c>
@@ -2243,8 +2377,11 @@
       <c r="G46" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B47" s="1" t="s">
         <v>109</v>
       </c>
@@ -2261,8 +2398,11 @@
       <c r="G47" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="2:7" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H47" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B48" s="1" t="s">
         <v>110</v>
       </c>
@@ -2279,8 +2419,11 @@
       <c r="G48" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="49" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H48" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B49" s="1" t="s">
         <v>111</v>
       </c>
@@ -2297,8 +2440,11 @@
       <c r="G49" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H49" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B50" s="11" t="s">
         <v>112</v>
       </c>
@@ -2315,8 +2461,11 @@
       <c r="G50" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="51" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H50" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B51" s="1" t="s">
         <v>115</v>
       </c>
@@ -2336,8 +2485,11 @@
       <c r="G51" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H51" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B52" s="1" t="s">
         <v>118</v>
       </c>
@@ -2356,8 +2508,11 @@
       <c r="G52" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H52" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B53" s="7" t="s">
         <v>120</v>
       </c>
@@ -2377,11 +2532,13 @@
       <c r="G53" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H53" s="5"/>
+      <c r="H53" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B54" s="1" t="s">
         <v>122</v>
       </c>
@@ -2398,8 +2555,11 @@
       <c r="G54" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="55" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H54" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B55" s="1" t="s">
         <v>123</v>
       </c>
@@ -2419,8 +2579,11 @@
       <c r="G55" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="56" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H55" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B56" s="1" t="s">
         <v>126</v>
       </c>
@@ -2437,11 +2600,13 @@
       <c r="G56" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H56" s="10"/>
+      <c r="H56" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I56" s="10"/>
       <c r="J56" s="10"/>
     </row>
-    <row r="57" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B57" s="1" t="s">
         <v>129</v>
       </c>
@@ -2456,8 +2621,11 @@
         <v>8</v>
       </c>
       <c r="G57" s="15"/>
-    </row>
-    <row r="58" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H57" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B58" s="1" t="s">
         <v>132</v>
       </c>
@@ -2474,8 +2642,11 @@
       <c r="G58" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H58" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B59" s="1" t="s">
         <v>133</v>
       </c>
@@ -2495,8 +2666,11 @@
       <c r="G59" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="60" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H59" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B60" s="1" t="s">
         <v>137</v>
       </c>
@@ -2513,8 +2687,11 @@
       <c r="G60" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="61" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H60" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B61" s="1" t="s">
         <v>140</v>
       </c>
@@ -2533,8 +2710,11 @@
       <c r="G61" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H61" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B62" s="1" t="s">
         <v>142</v>
       </c>
@@ -2549,8 +2729,11 @@
         <v>2</v>
       </c>
       <c r="G62" s="6"/>
-    </row>
-    <row r="63" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H62" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B63" s="1" t="s">
         <v>145</v>
       </c>
@@ -2565,8 +2748,11 @@
         <v>1</v>
       </c>
       <c r="G63" s="6"/>
-    </row>
-    <row r="64" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H63" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B64" s="1" t="s">
         <v>147</v>
       </c>
@@ -2585,8 +2771,11 @@
       <c r="G64" s="6" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="65" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H64" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B65" s="1" t="s">
         <v>151</v>
       </c>
@@ -2601,8 +2790,11 @@
         <v>1</v>
       </c>
       <c r="G65" s="6"/>
-    </row>
-    <row r="66" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H65" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B66" s="1" t="s">
         <v>153</v>
       </c>
@@ -2617,8 +2809,11 @@
         <v>1</v>
       </c>
       <c r="G66" s="6"/>
-    </row>
-    <row r="67" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H66" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B67" s="1" t="s">
         <v>155</v>
       </c>
@@ -2637,8 +2832,11 @@
       <c r="G67" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H67" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B68" s="1" t="s">
         <v>157</v>
       </c>
@@ -2657,8 +2855,11 @@
       <c r="G68" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="69" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H68" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B69" s="1" t="s">
         <v>159</v>
       </c>
@@ -2678,11 +2879,13 @@
       <c r="G69" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H69" s="5"/>
+      <c r="H69" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
     </row>
-    <row r="70" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B70" s="1" t="s">
         <v>161</v>
       </c>
@@ -2701,11 +2904,13 @@
       <c r="G70" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H70" s="10"/>
+      <c r="H70" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I70" s="10"/>
       <c r="J70" s="10"/>
     </row>
-    <row r="71" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B71" s="1" t="s">
         <v>163</v>
       </c>
@@ -2725,8 +2930,11 @@
       <c r="G71" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="72" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H71" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B72" s="1" t="s">
         <v>165</v>
       </c>
@@ -2745,8 +2953,11 @@
       <c r="G72" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="73" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H72" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B73" s="1" t="s">
         <v>166</v>
       </c>
@@ -2765,11 +2976,13 @@
       <c r="G73" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H73" s="5"/>
+      <c r="H73" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B74" s="1" t="s">
         <v>170</v>
       </c>
@@ -2786,11 +2999,13 @@
         <v>8</v>
       </c>
       <c r="G74" s="6"/>
-      <c r="H74" s="10"/>
+      <c r="H74" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I74" s="10"/>
       <c r="J74" s="10"/>
     </row>
-    <row r="75" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B75" s="1" t="s">
         <v>173</v>
       </c>
@@ -2809,8 +3024,11 @@
       <c r="G75" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="76" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H75" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B76" s="1" t="s">
         <v>175</v>
       </c>
@@ -2829,8 +3047,11 @@
       <c r="G76" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="77" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H76" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B77" s="7" t="s">
         <v>177</v>
       </c>
@@ -2847,8 +3068,11 @@
       <c r="G77" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="78" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H77" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B78" s="16" t="s">
         <v>179</v>
       </c>
@@ -2865,8 +3089,11 @@
       <c r="G78" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="79" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H78" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B79" s="1" t="s">
         <v>181</v>
       </c>
@@ -2886,8 +3113,11 @@
       <c r="G79" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="80" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H79" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B80" s="1" t="s">
         <v>185</v>
       </c>
@@ -2906,8 +3136,11 @@
       <c r="G80" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="81" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H80" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B81" s="16" t="s">
         <v>188</v>
       </c>
@@ -2924,11 +3157,13 @@
       <c r="G81" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H81" s="5"/>
+      <c r="H81" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
     </row>
-    <row r="82" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B82" s="1" t="s">
         <v>188</v>
       </c>
@@ -2945,11 +3180,13 @@
       <c r="G82" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H82" s="5"/>
+      <c r="H82" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
     </row>
-    <row r="83" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B83" s="7" t="s">
         <v>193</v>
       </c>
@@ -2969,11 +3206,13 @@
       <c r="G83" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H83" s="10"/>
+      <c r="H83" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I83" s="10"/>
       <c r="J83" s="10"/>
     </row>
-    <row r="84" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B84" s="7" t="s">
         <v>196</v>
       </c>
@@ -2992,11 +3231,13 @@
       <c r="G84" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H84" s="5"/>
+      <c r="H84" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I84" s="5"/>
       <c r="J84" s="5"/>
     </row>
-    <row r="85" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B85" s="7" t="s">
         <v>198</v>
       </c>
@@ -3015,11 +3256,13 @@
       <c r="G85" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H85" s="10"/>
+      <c r="H85" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I85" s="10"/>
       <c r="J85" s="10"/>
     </row>
-    <row r="86" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B86" s="7" t="s">
         <v>200</v>
       </c>
@@ -3036,11 +3279,13 @@
       <c r="G86" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H86" s="5"/>
+      <c r="H86" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I86" s="5"/>
       <c r="J86" s="5"/>
     </row>
-    <row r="87" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B87" s="7" t="s">
         <v>202</v>
       </c>
@@ -3059,8 +3304,11 @@
       <c r="G87" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="88" spans="2:10" s="10" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H87" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="88" spans="2:10" s="10" customFormat="1" ht="43.5" customHeight="1">
       <c r="B88" s="1" t="s">
         <v>204</v>
       </c>
@@ -3077,11 +3325,13 @@
       <c r="G88" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H88" s="5"/>
+      <c r="H88" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I88" s="5"/>
       <c r="J88" s="5"/>
     </row>
-    <row r="89" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B89" s="1" t="s">
         <v>206</v>
       </c>
@@ -3098,11 +3348,13 @@
       <c r="G89" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H89" s="10"/>
+      <c r="H89" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="I89" s="10"/>
       <c r="J89" s="10"/>
     </row>
-    <row r="90" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B90" s="7" t="s">
         <v>207</v>
       </c>
@@ -3121,8 +3373,11 @@
       <c r="G90" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="91" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H90" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="91" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B91" s="1" t="s">
         <v>211</v>
       </c>
@@ -3139,8 +3394,11 @@
       <c r="G91" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="92" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H91" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="92" spans="2:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B92" s="7" t="s">
         <v>214</v>
       </c>
@@ -3160,37 +3418,40 @@
         <v>8</v>
       </c>
       <c r="H92" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="93" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="B93" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="93" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="1" t="s">
+      <c r="C93" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F93" s="3">
         <v>24</v>
       </c>
       <c r="G93" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="94" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="B94" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="94" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="1" t="s">
+      <c r="C94" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F94" s="3">
         <v>10</v>
@@ -3198,13 +3459,16 @@
       <c r="G94" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="95" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H94" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="95" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B95" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="6" t="s">
@@ -3214,39 +3478,45 @@
         <v>1</v>
       </c>
       <c r="G95" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="H95" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="96" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="B96" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>226</v>
-      </c>
-    </row>
-    <row r="96" spans="2:10" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F96" s="3">
         <v>3</v>
       </c>
       <c r="G96" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="H96" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="B97" s="11" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="97" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="11" t="s">
+      <c r="C97" s="12" t="s">
         <v>230</v>
-      </c>
-      <c r="C97" s="12" t="s">
-        <v>231</v>
       </c>
       <c r="D97" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F97" s="12">
         <v>16</v>
@@ -3254,19 +3524,22 @@
       <c r="G97" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="98" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H97" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B98" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C98" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>234</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F98" s="9">
         <v>11</v>
@@ -3274,17 +3547,20 @@
       <c r="G98" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="99" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H98" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B99" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F99" s="3">
         <v>1</v>
@@ -3292,41 +3568,50 @@
       <c r="G99" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="100" spans="2:7" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H99" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" s="5" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B100" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="D100" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="E100" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="F100" s="6">
         <v>1</v>
       </c>
       <c r="G100" s="6"/>
-    </row>
-    <row r="101" spans="2:7" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H100" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="B101" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>244</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F101" s="3">
         <v>1</v>
       </c>
       <c r="G101" s="6" t="s">
         <v>8</v>
+      </c>
+      <c r="H101" s="5" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>